<commit_message>
golf updates and test project
</commit_message>
<xml_diff>
--- a/Golf/Results/course_history.xlsx
+++ b/Golf/Results/course_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikef\Documents\GitHub\Projects\Golf\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141795F-46A6-4886-8D53-E7A3F87CF90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73879709-32D2-4191-9BAB-40CBF0852D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{709062AC-F26C-481D-BE11-98E453AB4FDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{709062AC-F26C-481D-BE11-98E453AB4FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>event_name</t>
   </si>
@@ -221,6 +221,51 @@
   </si>
   <si>
     <t>Torrey Pines (South)</t>
+  </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>YDG</t>
+  </si>
+  <si>
+    <t>PAR 4/5 YDG</t>
+  </si>
+  <si>
+    <t>PAR 3 YDG</t>
+  </si>
+  <si>
+    <t>TOT</t>
+  </si>
+  <si>
+    <t>PAR 3</t>
+  </si>
+  <si>
+    <t>PAR 4</t>
+  </si>
+  <si>
+    <t>PAR 5</t>
+  </si>
+  <si>
+    <t>DIST</t>
+  </si>
+  <si>
+    <t>DIST SD</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>PUTT</t>
+  </si>
+  <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>OTT</t>
   </si>
 </sst>
 </file>
@@ -256,11 +301,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBCBBB1-1233-41B7-9217-F34025ACC21E}">
   <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A61" sqref="A60:A61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S78" sqref="S78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,17 +633,63 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +697,7 @@
         <v>43849</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -616,7 +708,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -627,7 +719,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -638,7 +730,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -649,7 +741,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -660,7 +752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -671,7 +763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -682,7 +774,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -693,7 +785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -702,7 +794,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -713,7 +805,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -724,7 +816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -735,7 +827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -743,7 +835,7 @@
         <v>44031</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1216,13 +1308,13 @@
       <c r="I67">
         <v>-3.93</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="4">
         <v>0.02</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="4">
         <v>-0.13</v>
       </c>
-      <c r="L67" s="2">
+      <c r="L67" s="4">
         <v>-0.63</v>
       </c>
       <c r="M67" s="2">
@@ -1273,13 +1365,13 @@
       <c r="I68" s="2">
         <v>-2.09</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="4">
         <v>-0.03</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="4">
         <v>-0.04</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68" s="4">
         <v>-0.71</v>
       </c>
       <c r="M68" s="2">
@@ -1312,6 +1404,9 @@
         <v>44584</v>
       </c>
       <c r="D69" s="2"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -1338,13 +1433,13 @@
       <c r="I70" s="2">
         <v>0.61</v>
       </c>
-      <c r="J70" s="2">
+      <c r="J70" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L70" s="2">
+      <c r="L70" s="4">
         <v>-0.26</v>
       </c>
       <c r="M70" s="2">
@@ -1395,13 +1490,13 @@
       <c r="I71" s="2">
         <v>-1.51</v>
       </c>
-      <c r="J71" s="2">
+      <c r="J71" s="4">
         <v>0.02</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="4">
         <v>-0.02</v>
       </c>
-      <c r="L71" s="2">
+      <c r="L71" s="4">
         <v>-0.34</v>
       </c>
       <c r="M71">
@@ -1452,13 +1547,13 @@
       <c r="I72" s="2">
         <v>-0.38</v>
       </c>
-      <c r="J72" s="2">
+      <c r="J72" s="4">
         <v>0.04</v>
       </c>
-      <c r="K72" s="2">
+      <c r="K72" s="4">
         <v>0.05</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="4">
         <v>-0.36</v>
       </c>
       <c r="M72" s="2">
@@ -1509,13 +1604,13 @@
       <c r="I73" s="2">
         <v>0.01</v>
       </c>
-      <c r="J73" s="2">
+      <c r="J73" s="4">
         <v>0.11</v>
       </c>
-      <c r="K73">
+      <c r="K73" s="4">
         <v>0.1</v>
       </c>
-      <c r="L73" s="2">
+      <c r="L73" s="4">
         <v>-0.53</v>
       </c>
       <c r="M73" s="2">
@@ -1566,13 +1661,13 @@
       <c r="I74" s="2">
         <v>1.29</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="4">
         <v>0.18</v>
       </c>
-      <c r="K74" s="2">
+      <c r="K74" s="4">
         <v>0.09</v>
       </c>
-      <c r="L74" s="2">
+      <c r="L74" s="4">
         <v>-0.28000000000000003</v>
       </c>
       <c r="M74" s="2">
@@ -1623,13 +1718,13 @@
       <c r="I75">
         <v>2.34</v>
       </c>
-      <c r="J75" s="2">
+      <c r="J75" s="4">
         <v>0.22</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="4">
         <v>0.25</v>
       </c>
-      <c r="L75" s="2">
+      <c r="L75" s="4">
         <v>-0.26</v>
       </c>
       <c r="M75">
@@ -1680,13 +1775,13 @@
       <c r="I76" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="4">
         <v>0.18</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="4">
         <v>-0.3</v>
       </c>
       <c r="M76">
@@ -1737,13 +1832,13 @@
       <c r="I77" s="2">
         <v>-0.71</v>
       </c>
-      <c r="J77" s="2">
+      <c r="J77" s="4">
         <v>0.03</v>
       </c>
-      <c r="K77">
+      <c r="K77" s="4">
         <v>0.05</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="4">
         <v>-0.31</v>
       </c>
       <c r="M77">
@@ -1777,6 +1872,9 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -1803,13 +1901,13 @@
       <c r="I79">
         <v>-0.24</v>
       </c>
-      <c r="J79">
+      <c r="J79" s="4">
         <v>0.05</v>
       </c>
-      <c r="K79">
+      <c r="K79" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L79">
+      <c r="L79" s="4">
         <v>-0.27</v>
       </c>
       <c r="M79">
@@ -1860,13 +1958,13 @@
       <c r="I80">
         <v>2.5</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="4">
         <v>0.19</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="4">
         <v>0.25</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="4">
         <v>-0.19</v>
       </c>
       <c r="M80">
@@ -1917,13 +2015,13 @@
       <c r="I81">
         <v>0.05</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="4">
         <v>0.17</v>
       </c>
-      <c r="K81">
+      <c r="K81" s="4">
         <v>0.03</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="4">
         <v>-0.32</v>
       </c>
       <c r="M81">

</xml_diff>